<commit_message>
modified picture to look more visually
</commit_message>
<xml_diff>
--- a/chart/gantt-chart.xlsx
+++ b/chart/gantt-chart.xlsx
@@ -45,7 +45,7 @@
     <t>Develop Front- End Application with Basic Template and Functionality</t>
   </si>
   <si>
-    <t>Duration in Months</t>
+    <t xml:space="preserve">Duration </t>
   </si>
 </sst>
 </file>
@@ -127,7 +127,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="35">
+  <cellStyleXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -163,8 +163,58 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -178,8 +228,9 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="35">
+  <cellStyles count="85">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -197,6 +248,31 @@
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -214,6 +290,31 @@
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -235,6 +336,10 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -246,186 +351,71 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$B$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Start Date</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>Duration (in Months)</c:v>
           </c:tx>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$2:$A$6</c:f>
-              <c:strCache>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$B$3:$C$7</c:f>
+              <c:multiLvlStrCache>
                 <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>Develop Front- End Application with Basic Template and Functionality</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Setup the back- end, HTTP Server</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Setup PostGreSQL Database Server</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Add User Authentication and Security</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Add Payment feature with PayPal</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>1-Apr</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>25-Mar</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>18-Mar</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>11-Feb</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>28-Jan</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Add Payment feature with PayPal</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Add User Authentication and Security</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Setup PostGreSQL Database Server</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Setup the back- end, HTTP Server</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Develop Front- End Application with Basic Template and Functionality</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$6</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>41667.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>41681.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>41716.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>41723.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>41730.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$C$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Duration in Months</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$2:$A$6</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>Develop Front- End Application with Basic Template and Functionality</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Setup the back- end, HTTP Server</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Setup PostGreSQL Database Server</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Add User Authentication and Security</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Add Payment feature with PayPal</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$C$2:$C$6</c:f>
+              <c:f>Sheet1!$D$3:$D$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>4.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.0</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$D$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>End Date</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$2:$A$6</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>Develop Front- End Application with Basic Template and Functionality</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Setup the back- end, HTTP Server</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Setup PostGreSQL Database Server</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Add User Authentication and Security</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Add Payment feature with PayPal</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$D$2:$D$6</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>41765.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>41765.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>41765.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>41765.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>41765.0</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -441,11 +431,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2109520840"/>
-        <c:axId val="2109197736"/>
+        <c:axId val="2105612168"/>
+        <c:axId val="2108555432"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2109520840"/>
+        <c:axId val="2105612168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -454,7 +444,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2109197736"/>
+        <c:crossAx val="2108555432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -462,18 +452,18 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2109197736"/>
+        <c:axId val="2108555432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="m/d/yy" sourceLinked="0"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2109520840"/>
+        <c:crossAx val="2105612168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -499,20 +489,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1625600</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>44450</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>660400</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>120650</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="11" name="Chart 10"/>
+        <xdr:cNvPr id="22" name="Chart 21"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -852,99 +842,102 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="B2:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="34.83203125" customWidth="1"/>
-    <col min="2" max="4" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" customWidth="1"/>
+    <col min="2" max="2" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="23">
-      <c r="A1" s="1" t="s">
+    <row r="2" spans="2:5" ht="23">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="54">
-      <c r="A2" s="3" t="s">
+    <row r="3" spans="2:5" ht="36">
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="5">
+        <v>41730</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+      <c r="E3" s="4">
+        <v>41765</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" ht="36">
+      <c r="B4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="5">
+        <v>41723</v>
+      </c>
+      <c r="D4" s="2">
+        <v>2</v>
+      </c>
+      <c r="E4" s="4">
+        <v>41765</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" ht="36">
+      <c r="B5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="5">
+        <v>41716</v>
+      </c>
+      <c r="D5" s="2">
+        <v>2</v>
+      </c>
+      <c r="E5" s="4">
+        <v>41765</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" ht="36">
+      <c r="B6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="5">
+        <v>41681</v>
+      </c>
+      <c r="D6" s="2">
+        <v>3</v>
+      </c>
+      <c r="E6" s="4">
+        <v>41765</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" ht="72">
+      <c r="B7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="4">
+      <c r="C7" s="5">
         <v>41667</v>
       </c>
-      <c r="C2" s="2">
-        <v>4</v>
-      </c>
-      <c r="D2" s="4">
-        <v>41765</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="18">
-      <c r="A3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="4">
-        <v>41681</v>
-      </c>
-      <c r="C3" s="2">
-        <v>3</v>
-      </c>
-      <c r="D3" s="4">
-        <v>41765</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="18">
-      <c r="A4" s="3" t="s">
+      <c r="D7" s="2">
         <v>5</v>
       </c>
-      <c r="B4" s="4">
-        <v>41716</v>
-      </c>
-      <c r="C4" s="2">
-        <v>2</v>
-      </c>
-      <c r="D4" s="4">
-        <v>41765</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="36">
-      <c r="A5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="4">
-        <v>41723</v>
-      </c>
-      <c r="C5" s="2">
-        <v>2</v>
-      </c>
-      <c r="D5" s="4">
-        <v>41765</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="18">
-      <c r="A6" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="4">
-        <v>41730</v>
-      </c>
-      <c r="C6" s="2">
-        <v>1</v>
-      </c>
-      <c r="D6" s="4">
+      <c r="E7" s="4">
         <v>41765</v>
       </c>
     </row>

</xml_diff>